<commit_message>
data cleaning/reorganization and summary figures of vegetation/seed bank to support resturcuturing of chapter outline (v2)
</commit_message>
<xml_diff>
--- a/2021_Seedlings_wider.xlsx
+++ b/2021_Seedlings_wider.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Thesis-related\2021_Field\MidIsland_Esutaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="14_{52E16CB1-BEF6-4DB0-82F3-09A76FBBF107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{49645CCE-1117-43D5-995D-011A9A6BAEEA}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="14_{52E16CB1-BEF6-4DB0-82F3-09A76FBBF107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{33A7F16D-2BF5-4E17-971B-3CECE8086DD9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{A3FDE5E4-45B0-493D-B596-F4BE77D90803}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{A3FDE5E4-45B0-493D-B596-F4BE77D90803}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,9 +479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D638CB-94AB-42C6-AFDD-4EDB6FD7F665}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y11" sqref="Y11"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,7 +564,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -576,34 +576,34 @@
         <v>44392</v>
       </c>
       <c r="E2" s="1">
-        <v>44458</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
+        <v>44461</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K2" s="2">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="L2" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M2" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="N2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -638,34 +638,34 @@
         <v>44392</v>
       </c>
       <c r="E3" s="1">
-        <v>44458</v>
-      </c>
-      <c r="F3" t="s">
+        <v>44461</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
       <c r="K3" s="2">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="L3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="N3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -700,31 +700,31 @@
         <v>44392</v>
       </c>
       <c r="E4" s="1">
-        <v>44458</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+        <v>44461</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="2">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -762,13 +762,13 @@
         <v>44392</v>
       </c>
       <c r="E5" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -777,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="N5" s="2">
         <v>0</v>
@@ -812,25 +812,25 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
         <v>44392</v>
       </c>
       <c r="E6" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
@@ -839,16 +839,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K6" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N6" s="2">
         <v>0</v>
@@ -869,51 +869,51 @@
         <v>0</v>
       </c>
       <c r="T6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>2016</v>
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>44392</v>
       </c>
       <c r="E7" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K7" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L7" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -931,27 +931,27 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>2016</v>
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>44392</v>
       </c>
       <c r="E8" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -960,22 +960,22 @@
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L8" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -998,37 +998,37 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9">
-        <v>2016</v>
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>44392</v>
       </c>
       <c r="E9" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9" s="2">
         <v>0</v>
@@ -1060,69 +1060,69 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>2016</v>
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <v>44392</v>
       </c>
       <c r="E10" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
         <v>2</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -1134,10 +1134,10 @@
         <v>44392</v>
       </c>
       <c r="E11" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1146,28 +1146,28 @@
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
       </c>
       <c r="M11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="2">
         <v>0</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1196,10 +1196,10 @@
         <v>44392</v>
       </c>
       <c r="E12" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -1208,31 +1208,31 @@
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2">
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M12" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
       </c>
       <c r="P12" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="2">
         <v>0</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -1258,10 +1258,10 @@
         <v>44392</v>
       </c>
       <c r="E13" s="1">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -1270,28 +1270,28 @@
         <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N13" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="2">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
@@ -1311,10 +1311,10 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>44392</v>
@@ -1323,7 +1323,7 @@
         <v>44458</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1332,22 +1332,22 @@
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2">
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
       </c>
       <c r="N14" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -1373,10 +1373,10 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
         <v>44392</v>
@@ -1385,31 +1385,31 @@
         <v>44458</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
       </c>
       <c r="M15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15" s="2">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
         <v>0</v>
@@ -1435,10 +1435,10 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
         <v>44392</v>
@@ -1446,29 +1446,29 @@
       <c r="E16" s="1">
         <v>44458</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>21</v>
+      <c r="F16" t="s">
+        <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2">
         <v>1</v>
       </c>
       <c r="M16" s="2">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="N16" s="2">
         <v>0</v>
@@ -1477,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="2">
         <v>0</v>
@@ -1496,11 +1496,11 @@
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17">
-        <v>2016</v>
+      <c r="B17" t="s">
+        <v>11</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
         <v>44392</v>
@@ -1518,19 +1518,19 @@
         <v>0</v>
       </c>
       <c r="I17" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2">
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="L17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M17" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N17" s="2">
         <v>2</v>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="2">
         <v>0</v>
@@ -1558,11 +1558,11 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
-        <v>2016</v>
+      <c r="B18" t="s">
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
         <v>44392</v>
@@ -1571,31 +1571,31 @@
         <v>44458</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="2">
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="L18" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M18" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="N18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O18" s="2">
         <v>0</v>
@@ -1633,10 +1633,10 @@
         <v>44458</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
@@ -1648,16 +1648,16 @@
         <v>0</v>
       </c>
       <c r="K19" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="L19" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M19" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="2">
         <v>0</v>
@@ -1695,28 +1695,28 @@
         <v>44458</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2">
         <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L20" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M20" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N20" s="2">
         <v>0</v>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="2">
         <v>0</v>
@@ -1757,28 +1757,28 @@
         <v>44458</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
       <c r="K21" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L21" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N21" s="2">
         <v>0</v>
@@ -1819,28 +1819,28 @@
         <v>44458</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>7</v>
-      </c>
       <c r="L22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M22" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N22" s="2">
         <v>0</v>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="2">
         <v>0</v>
@@ -1881,28 +1881,28 @@
         <v>44458</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
       </c>
       <c r="K23" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L23" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M23" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N23" s="2">
         <v>0</v>
@@ -1943,10 +1943,10 @@
         <v>44458</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -1958,16 +1958,16 @@
         <v>0</v>
       </c>
       <c r="K24" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="L24" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M24" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -1990,34 +1990,34 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>2016</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <v>44392</v>
       </c>
       <c r="E25" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="2">
         <v>3</v>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O25" s="2">
         <v>0</v>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="2">
         <v>0</v>
@@ -2047,51 +2047,51 @@
         <v>0</v>
       </c>
       <c r="T25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2016</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D26" s="1">
         <v>44392</v>
       </c>
       <c r="E26" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J26" s="2">
         <v>0</v>
       </c>
       <c r="K26" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L26" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
       </c>
       <c r="N26" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O26" s="2">
         <v>0</v>
@@ -2100,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="2">
         <v>0</v>
@@ -2114,55 +2114,55 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2016</v>
       </c>
       <c r="C27">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1">
         <v>44392</v>
       </c>
       <c r="E27" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
       <c r="I27" s="2">
+        <v>6</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2">
         <v>2</v>
       </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2">
-        <v>1</v>
-      </c>
       <c r="M27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O27" s="2">
         <v>0</v>
       </c>
       <c r="P27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="2">
         <v>0</v>
@@ -2176,46 +2176,46 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2016</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1">
         <v>44392</v>
       </c>
       <c r="E28" s="1">
-        <v>44461</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>21</v>
+        <v>44458</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28" s="2">
         <v>0</v>
       </c>
       <c r="K28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L28" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O28" s="2">
         <v>0</v>
@@ -2238,25 +2238,25 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>2016</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D29" s="1">
         <v>44392</v>
       </c>
       <c r="E29" s="1">
-        <v>44461</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>20</v>
+        <v>44458</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
@@ -2268,22 +2268,22 @@
         <v>0</v>
       </c>
       <c r="K29" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L29" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M29" s="2">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2">
         <v>2</v>
       </c>
-      <c r="N29" s="2">
-        <v>0</v>
-      </c>
       <c r="O29" s="2">
         <v>0</v>
       </c>
       <c r="P29" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q29" s="2">
         <v>0</v>
@@ -2295,57 +2295,57 @@
         <v>0</v>
       </c>
       <c r="T29" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>2016</v>
       </c>
       <c r="C30">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1">
         <v>44392</v>
       </c>
       <c r="E30" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
       </c>
       <c r="I30" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J30" s="2">
         <v>0</v>
       </c>
       <c r="K30" s="2">
+        <v>5</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2">
         <v>2</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2">
-        <v>5</v>
-      </c>
-      <c r="O30" s="2">
-        <v>0</v>
-      </c>
-      <c r="P30" s="2">
-        <v>0</v>
       </c>
       <c r="Q30" s="2">
         <v>0</v>
@@ -2362,52 +2362,52 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1">
         <v>44392</v>
       </c>
       <c r="E31" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J31" s="2">
         <v>0</v>
       </c>
       <c r="K31" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="2">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="N31" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O31" s="2">
         <v>0</v>
       </c>
       <c r="P31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="2">
         <v>0</v>
@@ -2424,46 +2424,46 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1">
         <v>44392</v>
       </c>
       <c r="E32" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J32" s="2">
         <v>0</v>
       </c>
       <c r="K32" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N32" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O32" s="2">
         <v>0</v>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T32" s="2">
         <v>0</v>
@@ -2486,58 +2486,58 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D33" s="1">
         <v>44392</v>
       </c>
       <c r="E33" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J33" s="2">
         <v>0</v>
       </c>
       <c r="K33" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="N33" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O33" s="2">
         <v>0</v>
       </c>
       <c r="P33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="2">
         <v>0</v>
       </c>
       <c r="R33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
@@ -2548,55 +2548,55 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1">
         <v>44392</v>
       </c>
       <c r="E34" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
       <c r="I34" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J34" s="2">
         <v>0</v>
       </c>
       <c r="K34" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L34" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M34" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="N34" s="2">
+        <v>3</v>
+      </c>
+      <c r="O34" s="2">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2">
         <v>2</v>
       </c>
-      <c r="O34" s="2">
-        <v>0</v>
-      </c>
-      <c r="P34" s="2">
-        <v>0</v>
-      </c>
       <c r="Q34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="2">
         <v>0</v>
@@ -2604,37 +2604,37 @@
       <c r="S34" s="2">
         <v>0</v>
       </c>
-      <c r="T34">
-        <v>3</v>
+      <c r="T34" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D35" s="1">
         <v>44392</v>
       </c>
       <c r="E35" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
       <c r="I35" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J35" s="2">
         <v>0</v>
@@ -2643,19 +2643,19 @@
         <v>2</v>
       </c>
       <c r="L35" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="N35" s="2">
         <v>5</v>
       </c>
-      <c r="N35" s="2">
-        <v>0</v>
-      </c>
       <c r="O35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q35" s="2">
         <v>0</v>
@@ -2667,36 +2667,36 @@
         <v>0</v>
       </c>
       <c r="T35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D36" s="1">
         <v>44392</v>
       </c>
       <c r="E36" s="1">
-        <v>44461</v>
+        <v>44458</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J36" s="2">
         <v>0</v>
@@ -2708,16 +2708,16 @@
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q36" s="2">
         <v>0</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
         <v>44392</v>
@@ -2749,60 +2749,60 @@
         <v>44461</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
       </c>
       <c r="I37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="2">
         <v>0</v>
       </c>
       <c r="K37" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="2">
+        <v>9</v>
+      </c>
+      <c r="N37" s="2">
+        <v>2</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>0</v>
+      </c>
+      <c r="R37" s="2">
+        <v>0</v>
+      </c>
+      <c r="S37" s="2">
+        <v>0</v>
+      </c>
+      <c r="T37">
         <v>3</v>
-      </c>
-      <c r="N37" s="2">
-        <v>3</v>
-      </c>
-      <c r="O37" s="2">
-        <v>0</v>
-      </c>
-      <c r="P37" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>0</v>
-      </c>
-      <c r="R37" s="2">
-        <v>0</v>
-      </c>
-      <c r="S37" s="2">
-        <v>0</v>
-      </c>
-      <c r="T37" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
         <v>44392</v>
@@ -2811,31 +2811,31 @@
         <v>44461</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
       <c r="I38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" s="2">
         <v>0</v>
       </c>
       <c r="K38" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
       </c>
       <c r="M38" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N38" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O38" s="2">
         <v>0</v>
@@ -2853,18 +2853,18 @@
         <v>0</v>
       </c>
       <c r="T38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
         <v>44392</v>
@@ -2873,16 +2873,16 @@
         <v>44461</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
       </c>
       <c r="I39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="2">
         <v>0</v>
@@ -2894,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39" s="2">
         <v>0</v>
@@ -2920,13 +2920,13 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <v>44392</v>
@@ -2935,31 +2935,31 @@
         <v>44461</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>8</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40" s="2">
         <v>19</v>
       </c>
-      <c r="H40" s="2">
-        <v>1</v>
-      </c>
-      <c r="I40" s="2">
-        <v>0</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1</v>
-      </c>
-      <c r="L40" s="2">
-        <v>0</v>
-      </c>
-      <c r="M40" s="2">
-        <v>0</v>
-      </c>
       <c r="N40" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O40" s="2">
         <v>0</v>
@@ -2982,13 +2982,13 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
         <v>44392</v>
@@ -2997,34 +2997,34 @@
         <v>44461</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
       <c r="I41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>7</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1</v>
+      </c>
+      <c r="M41" s="2">
+        <v>35</v>
+      </c>
+      <c r="N41" s="2">
         <v>3</v>
       </c>
-      <c r="K41" s="2">
-        <v>1</v>
-      </c>
-      <c r="L41" s="2">
-        <v>0</v>
-      </c>
-      <c r="M41" s="2">
-        <v>2</v>
-      </c>
-      <c r="N41" s="2">
-        <v>2</v>
-      </c>
       <c r="O41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P41" s="2">
         <v>0</v>
@@ -3039,18 +3039,18 @@
         <v>0</v>
       </c>
       <c r="T41" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D42" s="1">
         <v>44392</v>
@@ -3059,10 +3059,10 @@
         <v>44461</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
@@ -3074,22 +3074,22 @@
         <v>0</v>
       </c>
       <c r="K42" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
       </c>
       <c r="M42" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="N42" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O42" s="2">
         <v>0</v>
       </c>
       <c r="P42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q42" s="2">
         <v>0</v>
@@ -3106,13 +3106,13 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D43" s="1">
         <v>44392</v>
@@ -3133,19 +3133,19 @@
         <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N43" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O43" s="2">
         <v>0</v>
@@ -3168,13 +3168,13 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D44" s="1">
         <v>44392</v>
@@ -3192,51 +3192,51 @@
         <v>0</v>
       </c>
       <c r="I44" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K44" s="2">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2">
+        <v>1</v>
+      </c>
+      <c r="M44" s="2">
+        <v>2</v>
+      </c>
+      <c r="N44" s="2">
+        <v>0</v>
+      </c>
+      <c r="O44" s="2">
+        <v>0</v>
+      </c>
+      <c r="P44" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>0</v>
+      </c>
+      <c r="R44" s="2">
+        <v>0</v>
+      </c>
+      <c r="S44" s="2">
+        <v>0</v>
+      </c>
+      <c r="T44" s="2">
         <v>3</v>
-      </c>
-      <c r="L44" s="2">
-        <v>0</v>
-      </c>
-      <c r="M44" s="2">
-        <v>8</v>
-      </c>
-      <c r="N44" s="2">
-        <v>0</v>
-      </c>
-      <c r="O44" s="2">
-        <v>0</v>
-      </c>
-      <c r="P44" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>0</v>
-      </c>
-      <c r="R44" s="2">
-        <v>0</v>
-      </c>
-      <c r="S44" s="2">
-        <v>0</v>
-      </c>
-      <c r="T44" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D45" s="1">
         <v>44392</v>
@@ -3251,17 +3251,17 @@
         <v>19</v>
       </c>
       <c r="H45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="2">
         <v>0</v>
       </c>
       <c r="J45" s="2">
+        <v>0</v>
+      </c>
+      <c r="K45" s="2">
         <v>2</v>
       </c>
-      <c r="K45" s="2">
-        <v>0</v>
-      </c>
       <c r="L45" s="2">
         <v>0</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="N45" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O45" s="2">
         <v>0</v>
@@ -3292,13 +3292,13 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D46" s="1">
         <v>44392</v>
@@ -3319,19 +3319,19 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K46" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
       </c>
       <c r="M46" s="2">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O46" s="2">
         <v>0</v>
@@ -3340,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="2">
         <v>0</v>
@@ -3349,18 +3349,18 @@
         <v>0</v>
       </c>
       <c r="T46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D47" s="1">
         <v>44392</v>
@@ -3378,31 +3378,31 @@
         <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J47" s="2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K47" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L47" s="2">
         <v>1</v>
       </c>
       <c r="M47" s="2">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="N47" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O47" s="2">
         <v>0</v>
       </c>
       <c r="P47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="2">
         <v>0</v>
@@ -3411,18 +3411,18 @@
         <v>0</v>
       </c>
       <c r="T47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D48" s="1">
         <v>44392</v>
@@ -3440,22 +3440,22 @@
         <v>0</v>
       </c>
       <c r="I48" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J48" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K48" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="L48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="N48" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O48" s="2">
         <v>0</v>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="2">
         <v>0</v>
@@ -3473,25 +3473,22 @@
         <v>0</v>
       </c>
       <c r="T48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:T48">
+    <sortCondition ref="A2:A48"/>
+    <sortCondition ref="C2:C48"/>
+    <sortCondition ref="G2:G48"/>
+    <sortCondition ref="F2:F48"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -3720,6 +3717,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3727,14 +3733,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A30AD199-0DB8-4B61-B20E-5748A280BBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5242612F-23B4-48D4-B775-07A58CC91933}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3753,18 +3751,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A30AD199-0DB8-4B61-B20E-5748A280BBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C9DB3A2-5AF3-4303-AE63-937F08897BCF}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>